<commit_message>
Update para incluir mas stats
</commit_message>
<xml_diff>
--- a/input/eitc_municipal_2022.xlsx
+++ b/input/eitc_municipal_2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabriel/Documents/GitHub/Repos/Espacios-Abiertos/eitc-tableau/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34854EF4-B07F-544D-8447-C3B8A37C1FD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A75A10B-1D51-9741-AD2F-5413A01A701C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
   <si>
     <t>Municipios</t>
   </si>
@@ -348,6 +348,9 @@
   </si>
   <si>
     <t>Crédito por Trabajo - Promedio</t>
+  </si>
+  <si>
+    <t>OTROS*</t>
   </si>
 </sst>
 </file>
@@ -822,8 +825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA316"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D58" workbookViewId="0">
-      <selection activeCell="Z79" sqref="Z79"/>
+    <sheetView tabSelected="1" topLeftCell="K48" workbookViewId="0">
+      <selection activeCell="AA80" sqref="AA80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7623,33 +7626,90 @@
       </c>
     </row>
     <row r="80" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A80" s="1"/>
-      <c r="B80" s="2"/>
-      <c r="C80" s="2"/>
-      <c r="D80" s="2"/>
-      <c r="E80" s="2"/>
-      <c r="F80" s="2"/>
-      <c r="G80" s="2"/>
-      <c r="H80" s="2"/>
-      <c r="I80" s="2"/>
-      <c r="J80" s="2"/>
-      <c r="K80" s="2"/>
-      <c r="L80" s="2"/>
-      <c r="M80" s="2"/>
-      <c r="N80" s="2"/>
-      <c r="O80" s="2"/>
-      <c r="P80" s="2"/>
-      <c r="Q80" s="2"/>
-      <c r="R80" s="2"/>
-      <c r="S80" s="2"/>
-      <c r="T80" s="2"/>
-      <c r="U80" s="2"/>
-      <c r="V80" s="2"/>
-      <c r="W80" s="2"/>
-      <c r="X80" s="2"/>
-      <c r="Y80" s="3"/>
-      <c r="Z80" s="3"/>
-      <c r="AA80" s="3"/>
+      <c r="A80" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B80" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C80" s="2">
+        <v>75331438</v>
+      </c>
+      <c r="D80" s="2">
+        <v>4237</v>
+      </c>
+      <c r="E80" s="2">
+        <v>539244290</v>
+      </c>
+      <c r="F80" s="2">
+        <v>34497</v>
+      </c>
+      <c r="G80" s="2">
+        <v>93966012</v>
+      </c>
+      <c r="H80" s="2">
+        <v>4963</v>
+      </c>
+      <c r="I80" s="2">
+        <v>686141911</v>
+      </c>
+      <c r="J80" s="2">
+        <v>43410</v>
+      </c>
+      <c r="K80" s="2">
+        <v>644174855</v>
+      </c>
+      <c r="L80" s="2">
+        <v>38161</v>
+      </c>
+      <c r="M80" s="2">
+        <v>100242906</v>
+      </c>
+      <c r="N80" s="2">
+        <v>7700</v>
+      </c>
+      <c r="O80" s="2">
+        <v>35690162</v>
+      </c>
+      <c r="P80" s="2">
+        <v>3828</v>
+      </c>
+      <c r="Q80" s="2">
+        <v>780107923</v>
+      </c>
+      <c r="R80" s="2">
+        <v>48373</v>
+      </c>
+      <c r="S80" s="2">
+        <v>9683930</v>
+      </c>
+      <c r="T80" s="2">
+        <v>4963</v>
+      </c>
+      <c r="U80" s="2">
+        <v>69338977</v>
+      </c>
+      <c r="V80" s="2">
+        <v>43410</v>
+      </c>
+      <c r="W80" s="2">
+        <v>19800</v>
+      </c>
+      <c r="X80" s="2">
+        <v>13138</v>
+      </c>
+      <c r="Y80" s="3">
+        <f>Frame0[[#This Row],[Crédito por Trabajo - Casados]]+Frame0[[#This Row],[Crédito por Trabajo - Contribuyente Individual]]</f>
+        <v>79022907</v>
+      </c>
+      <c r="Z80" s="3">
+        <f>Frame0[[#This Row],[Planillas Casados - Crédito por Trabajo]]+Frame0[[#This Row],[Planillas Contribuyente Individual - Crédito por Trabajo]]</f>
+        <v>48373</v>
+      </c>
+      <c r="AA80" s="3">
+        <f>Frame0[[#This Row],[Crédito por Trabajo - Total]]/Frame0[[#This Row],[Planillas Total - Crédito por Trabajo]]</f>
+        <v>1633.6160047960639</v>
+      </c>
     </row>
     <row r="81" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A81" s="1"/>

</xml_diff>